<commit_message>
Added refactorings for 5.0.x
</commit_message>
<xml_diff>
--- a/docs/refactoring-4.0.x-to-4.1.0/Refactorings 4.0.x to 4.1.0.xlsx
+++ b/docs/refactoring-4.0.x-to-4.1.0/Refactorings 4.0.x to 4.1.0.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fries/Documents/Development/Repositories/finmath lib/doc/refactoring-4.0.x-to-4.1.0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fries/Documents/Development/Repositories/finmath lib/docs/refactoring-4.0.x-to-4.1.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A38D60DF-ED05-B24A-8D8F-224F3E561E07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFE8F19-94E9-C143-A246-328D1C5E11A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19980" xr2:uid="{89A50B95-A836-9647-8368-30876D9BFE05}"/>
+    <workbookView xWindow="7340" yWindow="460" windowWidth="33600" windowHeight="19980" xr2:uid="{89A50B95-A836-9647-8368-30876D9BFE05}"/>
   </bookViews>
   <sheets>
-    <sheet name="Refactorings 3.x to 4.x" sheetId="1" r:id="rId1"/>
+    <sheet name="Refactorings 4.0 to 4.1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -547,7 +547,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6EACCA-7E26-C148-ACB1-915E31E23464}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>